<commit_message>
test imputation on msband data
</commit_message>
<xml_diff>
--- a/HR_Data/LWP2_0015_lab_timing.xlsx
+++ b/HR_Data/LWP2_0015_lab_timing.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CDRIVE\CTPC\LIVEWELL WEARTECH WEARABILITY ALL\WEARTECH compiled participant timings with participant info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophie\Documents\MATLAB\HeartRate\HR_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -677,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,12 +692,14 @@
     <col min="5" max="5" width="26.7109375" customWidth="1"/>
     <col min="6" max="6" width="33.140625" customWidth="1"/>
     <col min="7" max="7" width="35" customWidth="1"/>
-    <col min="9" max="9" width="38" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="38" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>13</v>
       </c>
@@ -707,11 +709,11 @@
       <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -725,7 +727,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -741,14 +743,16 @@
       <c r="G3" s="5">
         <v>0.61681712962962965</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="K3" t="s">
         <v>68</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -764,14 +768,16 @@
       <c r="G4" s="5">
         <v>0.61707175925925928</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="K4" t="s">
         <v>69</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -787,14 +793,16 @@
       <c r="G5" s="6">
         <v>0.6173495370370371</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="K5" t="s">
         <v>70</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -813,14 +821,16 @@
       <c r="G6" s="5">
         <v>0.61762731481481481</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="K6" t="s">
         <v>71</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -839,17 +849,19 @@
       <c r="G7" s="5">
         <v>0.61790509259259252</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="K7" t="s">
         <v>72</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -868,17 +880,19 @@
       <c r="G8" s="5">
         <v>0.61815972222222226</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="L8" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>76</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -900,17 +914,19 @@
       <c r="G9" s="5">
         <v>0.61844907407407412</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="L9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>85</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -929,17 +945,19 @@
       <c r="G10" s="5">
         <v>0.61870370370370364</v>
       </c>
-      <c r="I10" t="s">
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="K10" t="s">
         <v>78</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>83</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -958,14 +976,16 @@
       <c r="G11" s="5">
         <v>0.61896990740740743</v>
       </c>
-      <c r="I11" t="s">
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="K11" t="s">
         <v>79</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -987,8 +1007,10 @@
       <c r="G12" s="5">
         <v>0.61928240740740736</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1007,11 +1029,13 @@
       <c r="G13" s="5">
         <v>0.61951388888888892</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="K13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1030,14 +1054,16 @@
       <c r="G14" s="5">
         <v>0.61978009259259259</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="K14" t="s">
         <v>88</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1059,14 +1085,16 @@
       <c r="G15" s="5">
         <v>0.62004629629629626</v>
       </c>
-      <c r="I15" t="s">
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="K15" t="s">
         <v>80</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1085,8 +1113,10 @@
       <c r="G16" s="5">
         <v>0.62031249999999993</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1105,8 +1135,10 @@
       <c r="G17" s="5">
         <v>0.62059027777777775</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1125,8 +1157,10 @@
       <c r="G18" s="5">
         <v>0.62085648148148154</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1148,8 +1182,10 @@
       <c r="G19" s="5">
         <v>0.62113425925925925</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1168,8 +1204,10 @@
       <c r="G20" s="5">
         <v>0.62138888888888888</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1188,8 +1226,10 @@
       <c r="G21" s="5">
         <v>0.62167824074074074</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1208,8 +1248,10 @@
       <c r="G22" s="5">
         <v>0.62193287037037037</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1231,8 +1273,10 @@
       <c r="G23" s="5">
         <v>0.62219907407407404</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1251,8 +1295,10 @@
       <c r="G24" s="5">
         <v>0.62246527777777783</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1268,8 +1314,10 @@
       <c r="G25" s="5">
         <v>0.62274305555555554</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>24</v>
       </c>
@@ -1279,8 +1327,10 @@
       <c r="G26" s="5">
         <v>0.62300925925925921</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1293,8 +1343,10 @@
       <c r="G27" s="5">
         <v>0.62327546296296299</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>26</v>
       </c>
@@ -1304,8 +1356,10 @@
       <c r="G28" s="5">
         <v>0.62355324074074081</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E29">
         <v>27</v>
       </c>
@@ -1315,8 +1369,10 @@
       <c r="G29" s="5">
         <v>0.62381944444444437</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>28</v>
       </c>
@@ -1326,6 +1382,8 @@
       <c r="G30" s="5">
         <v>0.62408564814814815</v>
       </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>